<commit_message>
Correção nas atividades de Login
</commit_message>
<xml_diff>
--- a/Data/Input/PLANILHA DE CONTROLE DE FATURAS.xlsx
+++ b/Data/Input/PLANILHA DE CONTROLE DE FATURAS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\robo\Projetos UiPath\prj_HC_ContasMunicipais\Data\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\robo\prj_HC_ContasMunicipais_SANASA\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE006A7-210D-42D8-8AA5-433CABD76021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC638D13-D59A-4007-8AAD-5E37D8DC0F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" firstSheet="4" activeTab="3" xr2:uid="{78ABD955-167D-4880-A8C2-036EBAA59347}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14055" activeTab="3" xr2:uid="{78ABD955-167D-4880-A8C2-036EBAA59347}"/>
   </bookViews>
   <sheets>
     <sheet name="CPFL TIME" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="189">
   <si>
     <t xml:space="preserve">Item </t>
   </si>
@@ -669,36 +669,6 @@
     <t>Água_HVC</t>
   </si>
   <si>
-    <t>RUA ONZE DE AGOSTO, 478 - CENTRO</t>
-  </si>
-  <si>
-    <t>RUA ONZE DE AGOSTO, 415</t>
-  </si>
-  <si>
-    <t>MEDPLEX</t>
-  </si>
-  <si>
-    <t>não</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Próprio </t>
-  </si>
-  <si>
-    <t>NÃO É DEB AUT 20784</t>
-  </si>
-  <si>
-    <t>NÃO É DEB AUT 20788</t>
-  </si>
-  <si>
-    <t>Agua_Jesuino Marcondes_278</t>
-  </si>
-  <si>
-    <t>Agua_Jesuino Marcondes_394</t>
-  </si>
-  <si>
-    <t>Agua_Jesuino Marcondes_400</t>
-  </si>
-  <si>
     <t>NRC</t>
   </si>
   <si>
@@ -799,7 +769,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000000000000"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -812,13 +782,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -906,12 +869,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1109,40 +1066,52 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1151,25 +1120,13 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1178,14 +1135,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1200,19 +1157,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1232,7 +1183,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1244,59 +1195,59 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1305,22 +1256,19 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1654,8 +1602,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0906FDB8-F0D8-4487-B754-C6C29A0BDEEC}" name="Tabela2" displayName="Tabela2" ref="A1:K15" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
-  <autoFilter ref="A1:K15" xr:uid="{0906FDB8-F0D8-4487-B754-C6C29A0BDEEC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0906FDB8-F0D8-4487-B754-C6C29A0BDEEC}" name="Tabela2" displayName="Tabela2" ref="A1:K3" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
+  <autoFilter ref="A1:K3" xr:uid="{0906FDB8-F0D8-4487-B754-C6C29A0BDEEC}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{66B4791A-4B42-4AA9-A656-F48FFD276222}" name="ITEM" dataDxfId="11">
       <calculatedColumnFormula>+A1+1</calculatedColumnFormula>
@@ -3816,7 +3764,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" location="/login" display="https://servicosonline.cpfl.com.br/agencia-webapp/ - /login" xr:uid="{0B3DF667-C25D-4804-81A0-494D56F1C290}"/>
     <hyperlink ref="G3" r:id="rId2" location="/login" display="https://servicosonline.cpfl.com.br/agencia-webapp/ - /login" xr:uid="{B61B878F-83E9-4635-88C8-1A936F3EED8E}"/>
@@ -6023,7 +5971,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://app.sanasa.com.br/vagencic4/app?hptAppId=FR902P&amp;hptExec=Y" xr:uid="{C70B5D69-94C1-421C-935D-3E7F40B698A7}"/>
     <hyperlink ref="I3:I57" r:id="rId2" display="https://app.sanasa.com.br/vagencic4/app?hptAppId=FR902P&amp;hptExec=Y" xr:uid="{6B279AE2-9CEB-45E2-9B75-11245AA1A5F7}"/>
@@ -6050,13 +5998,13 @@
     <col min="4" max="4" width="18.85546875" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="57" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="34" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45.42578125" style="34" customWidth="1"/>
-    <col min="9" max="9" width="29" style="34" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" style="42" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25" style="42" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="30.140625" style="42" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" style="34" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.42578125" style="32" customWidth="1"/>
+    <col min="9" max="9" width="29" style="32" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25" style="40" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" style="40" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" style="32" hidden="1" customWidth="1"/>
     <col min="14" max="15" width="32.140625" customWidth="1"/>
     <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="1018" width="9.140625" customWidth="1"/>
@@ -6081,175 +6029,175 @@
       <c r="F1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="M1" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="N1" s="49" t="s">
+      <c r="N1" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="49" t="s">
+      <c r="O1" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="P1" s="49" t="s">
+      <c r="P1" s="47" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+    <row r="2" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="38">
+      <c r="C2" s="36">
         <v>1</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38" t="s">
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="H2" s="37">
+      <c r="H2" s="35">
         <v>20335</v>
       </c>
-      <c r="I2" s="37" t="s">
+      <c r="I2" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="J2" s="37">
+      <c r="J2" s="35">
         <v>7989288</v>
       </c>
-      <c r="K2" s="37" t="s">
+      <c r="K2" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="L2" s="51">
+      <c r="L2" s="49">
         <v>310003443279</v>
       </c>
-      <c r="M2" s="37">
+      <c r="M2" s="35">
         <v>43936</v>
       </c>
-      <c r="N2" s="37" t="s">
+      <c r="N2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="67">
+      <c r="O2" s="65">
         <f>J2</f>
         <v>7989288</v>
       </c>
-      <c r="P2" s="67" t="s">
+      <c r="P2" s="65" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+    <row r="3" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="36">
         <v>1</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38" t="s">
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="H3" s="37">
+      <c r="H3" s="35">
         <v>20152</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="I3" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="J3" s="37">
+      <c r="J3" s="35">
         <v>8469636</v>
       </c>
-      <c r="K3" s="37" t="s">
+      <c r="K3" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="L3" s="51">
+      <c r="L3" s="49">
         <v>310003443960</v>
       </c>
-      <c r="M3" s="37">
+      <c r="M3" s="35">
         <v>43970</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="N3" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="67">
+      <c r="O3" s="65">
         <f t="shared" ref="O3:O15" si="0">J3</f>
         <v>8469636</v>
       </c>
-      <c r="P3" s="67" t="s">
+      <c r="P3" s="65" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="36">
         <v>1</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38" t="s">
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="G4" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="H4" s="37">
+      <c r="H4" s="35">
         <v>20352</v>
       </c>
-      <c r="I4" s="37" t="s">
+      <c r="I4" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="J4" s="37">
+      <c r="J4" s="35">
         <v>8469512</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="L4" s="51">
+      <c r="L4" s="49">
         <v>310003443627</v>
       </c>
-      <c r="M4" s="37">
+      <c r="M4" s="35">
         <v>43909</v>
       </c>
-      <c r="N4" s="37" t="s">
+      <c r="N4" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="67">
+      <c r="O4" s="65">
         <f t="shared" si="0"/>
         <v>8469512</v>
       </c>
-      <c r="P4" s="67" t="s">
+      <c r="P4" s="65" t="s">
         <v>13</v>
       </c>
     </row>
@@ -6268,407 +6216,407 @@
       <c r="F5" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="H5" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="I5" s="37" t="s">
+      <c r="I5" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="J5" s="37">
+      <c r="J5" s="35">
         <v>42235685</v>
       </c>
-      <c r="K5" s="37" t="s">
+      <c r="K5" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="L5" s="51">
+      <c r="L5" s="49">
         <v>320001249880</v>
       </c>
-      <c r="M5" s="37">
+      <c r="M5" s="35">
         <v>43966</v>
       </c>
-      <c r="N5" s="37" t="s">
+      <c r="N5" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="67">
+      <c r="O5" s="65">
         <f t="shared" si="0"/>
         <v>42235685</v>
       </c>
-      <c r="P5" s="67" t="s">
+      <c r="P5" s="65" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+    <row r="6" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="36">
         <v>2</v>
       </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38" t="s">
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="I6" s="37" t="s">
+      <c r="I6" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="J6" s="37">
+      <c r="J6" s="35">
         <v>8239738</v>
       </c>
-      <c r="K6" s="37" t="s">
+      <c r="K6" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="L6" s="51">
+      <c r="L6" s="49">
         <v>320000079654</v>
       </c>
-      <c r="M6" s="37">
+      <c r="M6" s="35">
         <v>43966</v>
       </c>
-      <c r="N6" s="37" t="s">
+      <c r="N6" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="O6" s="67">
+      <c r="O6" s="65">
         <f t="shared" si="0"/>
         <v>8239738</v>
       </c>
-      <c r="P6" s="67" t="s">
+      <c r="P6" s="65" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+    <row r="7" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="36">
         <v>1</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38" t="s">
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="G7" s="37" t="s">
+      <c r="G7" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="H7" s="37">
+      <c r="H7" s="35">
         <v>20470</v>
       </c>
-      <c r="I7" s="37" t="s">
+      <c r="I7" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="J7" s="37">
+      <c r="J7" s="35">
         <v>9024859</v>
       </c>
-      <c r="K7" s="37" t="s">
+      <c r="K7" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="L7" s="51">
+      <c r="L7" s="49">
         <v>310003444046</v>
       </c>
-      <c r="M7" s="37">
+      <c r="M7" s="35">
         <v>43944</v>
       </c>
-      <c r="N7" s="37" t="s">
+      <c r="N7" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="67">
+      <c r="O7" s="65">
         <f t="shared" si="0"/>
         <v>9024859</v>
       </c>
-      <c r="P7" s="67" t="s">
+      <c r="P7" s="65" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="36">
         <v>1</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38" t="s">
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="I8" s="37" t="s">
+      <c r="I8" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="J8" s="37">
+      <c r="J8" s="35">
         <v>41965930</v>
       </c>
-      <c r="K8" s="37" t="s">
+      <c r="K8" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="L8" s="51">
+      <c r="L8" s="49">
         <v>310003444275</v>
       </c>
-      <c r="M8" s="37">
+      <c r="M8" s="35">
         <v>43913</v>
       </c>
-      <c r="N8" s="37" t="s">
+      <c r="N8" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="67">
+      <c r="O8" s="65">
         <f t="shared" si="0"/>
         <v>41965930</v>
       </c>
-      <c r="P8" s="67" t="s">
+      <c r="P8" s="65" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+    <row r="9" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="36">
         <v>1</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38">
+      <c r="D9" s="36"/>
+      <c r="E9" s="36">
         <v>3322</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="G9" s="37" t="s">
+      <c r="G9" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="37" t="s">
+      <c r="H9" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="I9" s="37" t="s">
+      <c r="I9" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="J9" s="37">
+      <c r="J9" s="35">
         <v>9024891</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="L9" s="51">
+      <c r="L9" s="49">
         <v>320001259575</v>
       </c>
-      <c r="M9" s="37">
+      <c r="M9" s="35">
         <v>43957</v>
       </c>
-      <c r="N9" s="37" t="s">
+      <c r="N9" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="O9" s="67">
+      <c r="O9" s="65">
         <f t="shared" si="0"/>
         <v>9024891</v>
       </c>
-      <c r="P9" s="67" t="s">
+      <c r="P9" s="65" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+    <row r="10" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="36">
         <v>1</v>
       </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38" t="s">
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="G10" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="I10" s="37" t="s">
+      <c r="I10" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="J10" s="37">
+      <c r="J10" s="35">
         <v>9024905</v>
       </c>
-      <c r="K10" s="37" t="s">
+      <c r="K10" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="L10" s="51">
+      <c r="L10" s="49">
         <v>310042493389</v>
       </c>
-      <c r="M10" s="37">
+      <c r="M10" s="35">
         <v>43913</v>
       </c>
-      <c r="N10" s="37" t="s">
+      <c r="N10" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="O10" s="67">
+      <c r="O10" s="65">
         <f t="shared" si="0"/>
         <v>9024905</v>
       </c>
-      <c r="P10" s="67" t="s">
+      <c r="P10" s="65" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+    <row r="11" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="36">
         <v>1</v>
       </c>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38">
+      <c r="D11" s="36"/>
+      <c r="E11" s="36">
         <v>3314</v>
       </c>
-      <c r="F11" s="38" t="s">
+      <c r="F11" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="H11" s="37">
+      <c r="H11" s="35">
         <v>20722</v>
       </c>
-      <c r="I11" s="37" t="s">
+      <c r="I11" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="J11" s="37">
+      <c r="J11" s="35">
         <v>9024867</v>
       </c>
-      <c r="K11" s="37" t="s">
+      <c r="K11" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="L11" s="51">
+      <c r="L11" s="49">
         <v>310077670820</v>
       </c>
-      <c r="M11" s="37">
+      <c r="M11" s="35">
         <v>43913</v>
       </c>
-      <c r="N11" s="37" t="s">
+      <c r="N11" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="O11" s="67">
+      <c r="O11" s="65">
         <f t="shared" si="0"/>
         <v>9024867</v>
       </c>
-      <c r="P11" s="67" t="s">
+      <c r="P11" s="65" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+    <row r="12" spans="1:16" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="C12" s="38">
+      <c r="C12" s="36">
         <v>1</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38" t="s">
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="G12" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="H12" s="37">
+      <c r="H12" s="35">
         <v>20791</v>
       </c>
-      <c r="I12" s="37" t="s">
+      <c r="I12" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="J12" s="37">
+      <c r="J12" s="35">
         <v>8403686</v>
       </c>
-      <c r="K12" s="37" t="s">
+      <c r="K12" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="L12" s="51">
+      <c r="L12" s="49">
         <v>310003443414</v>
       </c>
-      <c r="M12" s="37">
+      <c r="M12" s="35">
         <v>43913</v>
       </c>
-      <c r="N12" s="37" t="s">
+      <c r="N12" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="O12" s="67">
+      <c r="O12" s="65">
         <f t="shared" si="0"/>
         <v>8403686</v>
       </c>
-      <c r="P12" s="67" t="s">
+      <c r="P12" s="65" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30"/>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="37" t="s">
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="H13" s="37">
+      <c r="H13" s="35">
         <v>20158</v>
       </c>
-      <c r="I13" s="37" t="s">
+      <c r="I13" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="J13" s="37">
+      <c r="J13" s="35">
         <v>4002719386</v>
       </c>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37" t="s">
+      <c r="K13" s="35"/>
+      <c r="L13" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="M13" s="37">
+      <c r="M13" s="35">
         <v>43945</v>
       </c>
-      <c r="N13" s="37" t="s">
+      <c r="N13" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="O13" s="67">
+      <c r="O13" s="65">
         <f t="shared" si="0"/>
         <v>4002719386</v>
       </c>
-      <c r="P13" s="67" t="s">
+      <c r="P13" s="65" t="s">
         <v>13</v>
       </c>
     </row>
@@ -6676,7 +6624,7 @@
       <c r="A14" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="37" t="s">
         <v>134</v>
       </c>
       <c r="C14" s="27">
@@ -6687,132 +6635,132 @@
       <c r="F14" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="G14" s="37" t="s">
+      <c r="G14" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="H14" s="37" t="s">
+      <c r="H14" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="I14" s="37" t="s">
+      <c r="I14" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="J14" s="37">
+      <c r="J14" s="35">
         <v>4002696810</v>
       </c>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37" t="s">
+      <c r="K14" s="35"/>
+      <c r="L14" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="M14" s="37">
+      <c r="M14" s="35">
         <v>43955</v>
       </c>
-      <c r="N14" s="37" t="s">
+      <c r="N14" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="O14" s="67">
+      <c r="O14" s="65">
         <f t="shared" si="0"/>
         <v>4002696810</v>
       </c>
-      <c r="P14" s="67" t="s">
+      <c r="P14" s="65" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="30"/>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="37" t="s">
         <v>137</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
       <c r="F15" s="27"/>
-      <c r="G15" s="37" t="s">
+      <c r="G15" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="H15" s="37">
+      <c r="H15" s="35">
         <v>20788</v>
       </c>
-      <c r="I15" s="37" t="s">
+      <c r="I15" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="J15" s="37">
+      <c r="J15" s="35">
         <v>32553048</v>
       </c>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37" t="s">
+      <c r="K15" s="35"/>
+      <c r="L15" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37" t="s">
+      <c r="M15" s="35"/>
+      <c r="N15" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="O15" s="67">
+      <c r="O15" s="65">
         <f t="shared" si="0"/>
         <v>32553048</v>
       </c>
-      <c r="P15" s="67" t="s">
+      <c r="P15" s="65" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30"/>
-      <c r="B16" s="39"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="27"/>
       <c r="D16" s="27"/>
       <c r="E16" s="27"/>
       <c r="F16" s="27"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="34"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="32"/>
     </row>
     <row r="17" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="30"/>
-      <c r="B17" s="39"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
       <c r="F17" s="27"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="34"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="32"/>
     </row>
     <row r="18" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="30"/>
-      <c r="B18" s="39"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
       <c r="E18" s="27"/>
       <c r="F18" s="27"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="34"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="32"/>
     </row>
     <row r="19" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30"/>
-      <c r="B19" s="38"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="27"/>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
       <c r="F19" s="27"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="34"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="32"/>
     </row>
     <row r="20" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
@@ -6828,16 +6776,16 @@
       <c r="E20" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="F20" s="41" t="s">
+      <c r="F20" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="34"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="32"/>
     </row>
     <row r="21" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
@@ -6853,16 +6801,16 @@
       <c r="E21" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="F21" s="41" t="s">
+      <c r="F21" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="34"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="32"/>
     </row>
     <row r="22" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
@@ -6878,16 +6826,16 @@
       <c r="E22" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="F22" s="41" t="s">
+      <c r="F22" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="34"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="32"/>
     </row>
     <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
@@ -6895,30 +6843,30 @@
       <c r="A25" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="B25" s="38" t="s">
+      <c r="B25" s="36" t="s">
         <v>148</v>
       </c>
-      <c r="C25" s="38">
+      <c r="C25" s="36">
         <v>1</v>
       </c>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38" t="s">
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="34"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="32"/>
     </row>
     <row r="26" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="36" t="s">
         <v>150</v>
       </c>
       <c r="C26" s="27">
@@ -6929,37 +6877,37 @@
       <c r="F26" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="34"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="32"/>
     </row>
     <row r="72" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G72" s="44"/>
-      <c r="H72" s="45">
+      <c r="G72" s="42"/>
+      <c r="H72" s="43">
         <v>20784</v>
       </c>
-      <c r="I72" s="45"/>
-      <c r="J72" s="46" t="s">
+      <c r="I72" s="43"/>
+      <c r="J72" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="K72" s="46"/>
-      <c r="L72" s="46"/>
-      <c r="M72" s="45"/>
+      <c r="K72" s="44"/>
+      <c r="L72" s="44"/>
+      <c r="M72" s="43"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="36"/>
-      <c r="B85" s="36"/>
-      <c r="C85" s="36"/>
-      <c r="D85" s="36"/>
-      <c r="E85" s="36"/>
-      <c r="F85" s="36"/>
+      <c r="A85" s="34"/>
+      <c r="B85" s="34"/>
+      <c r="C85" s="34"/>
+      <c r="D85" s="34"/>
+      <c r="E85" s="34"/>
+      <c r="F85" s="34"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B1:G1 I1:P1">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
@@ -6977,10 +6925,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C2AEC7-8CDD-4965-8DAA-F0648576B946}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6989,9 +6937,9 @@
     <col min="2" max="2" width="55" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="32" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="42.140625" customWidth="1"/>
     <col min="9" max="9" width="49" customWidth="1"/>
     <col min="10" max="10" width="20.85546875" bestFit="1" customWidth="1"/>
@@ -7023,13 +6971,13 @@
       <c r="H1" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="K1" s="33" t="s">
         <v>7</v>
       </c>
     </row>
@@ -7058,23 +7006,23 @@
       <c r="H2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="65">
+      <c r="J2" s="63">
         <v>917526</v>
       </c>
-      <c r="K2" s="66">
+      <c r="K2" s="64">
         <v>46009718000140</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21">
-        <f>+A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>129</v>
+      <c r="A3" s="21" t="e">
+        <f>+#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="C3" s="29" t="s">
         <v>109</v>
@@ -7083,503 +7031,57 @@
         <v>100</v>
       </c>
       <c r="E3" s="30">
-        <v>20791</v>
+        <v>20335</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>101</v>
       </c>
       <c r="G3" s="30">
-        <v>50781</v>
+        <v>909986</v>
       </c>
       <c r="H3" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="64" t="s">
+      <c r="I3" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="67">
-        <v>50781</v>
-      </c>
-      <c r="K3" s="66">
+      <c r="J3" s="65">
+        <v>909986</v>
+      </c>
+      <c r="K3" s="64">
         <v>46009718000140</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
-        <f t="shared" ref="A4:A15" si="0">+A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="E4" s="30">
-        <v>20352</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="G4" s="30">
-        <v>56432</v>
-      </c>
-      <c r="H4" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="67">
-        <v>56432</v>
-      </c>
-      <c r="K4" s="66">
-        <v>46009718000301</v>
-      </c>
+      <c r="D4"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
     </row>
     <row r="5" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="30">
-        <v>20626</v>
-      </c>
-      <c r="F5" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="G5" s="30">
-        <v>4046843</v>
-      </c>
-      <c r="H5" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" s="67">
-        <v>4046843</v>
-      </c>
-      <c r="K5" s="66">
-        <v>46009718000140</v>
-      </c>
+      <c r="D5"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="E6" s="30">
-        <v>20152</v>
-      </c>
-      <c r="F6" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="G6" s="33">
-        <v>56580</v>
-      </c>
-      <c r="H6" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="68">
-        <v>56580</v>
-      </c>
-      <c r="K6" s="66">
-        <v>46009718000140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="E7" s="30">
-        <v>20788</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="G7" s="30">
-        <v>56473</v>
-      </c>
-      <c r="H7" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="67">
-        <v>56473</v>
-      </c>
-      <c r="K7" s="66">
-        <v>11457797000177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>162</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="F8" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="G8" s="30">
-        <v>4370359</v>
-      </c>
-      <c r="H8" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="67">
-        <v>4370359</v>
-      </c>
-      <c r="K8" s="66">
-        <v>46009718000140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>162</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>164</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="G9" s="30">
-        <v>56564</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="67">
-        <v>56564</v>
-      </c>
-      <c r="K9" s="66">
-        <v>46009718000140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="G10" s="30">
-        <v>3208410</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="67">
-        <v>3208410</v>
-      </c>
-      <c r="K10" s="66">
-        <v>46009718000140</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>166</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="G11" s="30">
-        <v>454819</v>
-      </c>
-      <c r="H11" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="67">
-        <v>454819</v>
-      </c>
-      <c r="K11" s="66">
-        <v>46009718000140</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>167</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="G12" s="30">
-        <v>454835</v>
-      </c>
-      <c r="H12" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="67">
-        <v>454835</v>
-      </c>
-      <c r="K12" s="66">
-        <v>46009718000140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="E13" s="33">
-        <v>20470</v>
-      </c>
-      <c r="F13" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="G13" s="33">
-        <v>3139110</v>
-      </c>
-      <c r="H13" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="68">
-        <v>3139110</v>
-      </c>
-      <c r="K13" s="66">
-        <v>46009718000140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="E14" s="30">
-        <v>20722</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="G14" s="30">
-        <v>4311361</v>
-      </c>
-      <c r="H14" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="67">
-        <v>4311361</v>
-      </c>
-      <c r="K14" s="66">
-        <v>46009718000140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="E15" s="30">
-        <v>20335</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="G15" s="30">
-        <v>909986</v>
-      </c>
-      <c r="H15" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="67">
-        <v>909986</v>
-      </c>
-      <c r="K15" s="66">
-        <v>46009718000140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D16"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-    </row>
-    <row r="17" spans="4:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D17"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-    </row>
-    <row r="18" spans="4:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D18"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
+      <c r="D6"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://app.sanasa.com.br/vagencic4/app?hptAppId=FR902P&amp;hptExec=Y" xr:uid="{9FD859E2-CB74-44A5-B9EB-07009B04F7BE}"/>
-    <hyperlink ref="I3" r:id="rId2" display="https://app.sanasa.com.br/vagencic4/app?hptAppId=FR902P&amp;hptExec=Y" xr:uid="{CEAC0A30-2128-4E5E-9357-3F6A94913D22}"/>
-    <hyperlink ref="I4" r:id="rId3" display="https://app.sanasa.com.br/vagencic4/app?hptAppId=FR902P&amp;hptExec=Y" xr:uid="{F6BBBB4C-73A7-45D7-9014-EBD8DF0A7B04}"/>
-    <hyperlink ref="I5" r:id="rId4" display="https://app.sanasa.com.br/vagencic4/app?hptAppId=FR902P&amp;hptExec=Y" xr:uid="{AD0329F6-AA2A-4DE7-8BA3-2685F91FE3F9}"/>
-    <hyperlink ref="I6" r:id="rId5" display="https://app.sanasa.com.br/vagencic4/app?hptAppId=FR902P&amp;hptExec=Y" xr:uid="{02BF094C-9DB5-4040-A901-EE97AA2C9E93}"/>
-    <hyperlink ref="I7" r:id="rId6" display="https://app.sanasa.com.br/vagencic4/app?hptAppId=FR902P&amp;hptExec=Y" xr:uid="{2448AD26-9BC7-4B56-9968-B69D5B8E2D8D}"/>
-    <hyperlink ref="I8" r:id="rId7" display="https://app.sanasa.com.br/vagencic4/app?hptAppId=FR902P&amp;hptExec=Y" xr:uid="{564AEB4A-4426-48D5-B3CA-F06430C88002}"/>
-    <hyperlink ref="I9" r:id="rId8" display="https://app.sanasa.com.br/vagencic4/app?hptAppId=FR902P&amp;hptExec=Y" xr:uid="{7B92B465-211D-4E3D-81CD-93DF8C655BAD}"/>
-    <hyperlink ref="I10" r:id="rId9" display="https://app.sanasa.com.br/vagencic4/app?hptAppId=FR902P&amp;hptExec=Y" xr:uid="{9A926B2B-BB3E-4DBB-B8CE-D113ECF51489}"/>
-    <hyperlink ref="I11" r:id="rId10" display="https://app.sanasa.com.br/vagencic4/app?hptAppId=FR902P&amp;hptExec=Y" xr:uid="{24CC5A65-B7B6-407F-92A3-F4C658A3659F}"/>
-    <hyperlink ref="I12" r:id="rId11" display="https://app.sanasa.com.br/vagencic4/app?hptAppId=FR902P&amp;hptExec=Y" xr:uid="{D45BB4CA-336F-419F-9A73-D824C4E9160A}"/>
-    <hyperlink ref="I13" r:id="rId12" display="https://app.sanasa.com.br/vagencic4/app?hptAppId=FR902P&amp;hptExec=Y" xr:uid="{A1244916-3DB3-47AA-85B0-C53F8FA10467}"/>
-    <hyperlink ref="I14" r:id="rId13" display="https://app.sanasa.com.br/vagencic4/app?hptAppId=FR902P&amp;hptExec=Y" xr:uid="{ACCF263B-DEA2-4F26-B99E-D339FDF41EE9}"/>
-    <hyperlink ref="I15" r:id="rId14" display="https://app.sanasa.com.br/vagencic4/app?hptAppId=FR902P&amp;hptExec=Y" xr:uid="{3D28804D-8062-4CA7-97DB-93F1333A00B1}"/>
-    <hyperlink ref="H2" r:id="rId15" xr:uid="{3EEEA03A-690E-4CC7-BA3B-1E12F72898D4}"/>
-    <hyperlink ref="H3" r:id="rId16" xr:uid="{95409C08-14EE-421A-9451-7B1B6275CF79}"/>
-    <hyperlink ref="H4" r:id="rId17" xr:uid="{AE2B8C65-E8FA-4F38-AB2D-9F2CE65C756E}"/>
-    <hyperlink ref="H5:H6" r:id="rId18" display="Centraldenotas.cshc@hospitalcare.com.br" xr:uid="{72249653-9F40-480A-9525-4F8FD10F4E42}"/>
-    <hyperlink ref="H7" r:id="rId19" xr:uid="{1EB3BB78-8185-4A96-8EC0-DAAAD6E45298}"/>
-    <hyperlink ref="H8:H9" r:id="rId20" display="Centraldenotas.cshc@hospitalcare.com.br" xr:uid="{E4D2A215-7464-4F8C-8B65-340CE98C64AE}"/>
-    <hyperlink ref="H9" r:id="rId21" xr:uid="{47092953-6257-4ADE-8C01-B835A6A90191}"/>
-    <hyperlink ref="H10:H15" r:id="rId22" display="Centraldenotas.cshc@hospitalcare.com.br" xr:uid="{1A255940-DF20-4E8C-8D97-C5DAEC5ECBF4}"/>
+    <hyperlink ref="I3" r:id="rId2" display="https://app.sanasa.com.br/vagencic4/app?hptAppId=FR902P&amp;hptExec=Y" xr:uid="{3D28804D-8062-4CA7-97DB-93F1333A00B1}"/>
+    <hyperlink ref="H2" r:id="rId3" xr:uid="{3EEEA03A-690E-4CC7-BA3B-1E12F72898D4}"/>
+    <hyperlink ref="H3" r:id="rId4" xr:uid="{1A255940-DF20-4E8C-8D97-C5DAEC5ECBF4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId24"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7596,614 +7098,614 @@
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="62" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" style="62" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="60" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" style="60" customWidth="1"/>
     <col min="5" max="5" width="43.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18" style="62" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" style="62" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="62"/>
+    <col min="6" max="6" width="18" style="60" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" style="60" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="60"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="50" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="53" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="61" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="61" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="61" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="54">
+        <v>9464051154</v>
+      </c>
+      <c r="B2" s="66">
+        <v>20470</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="56">
+        <v>202101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="55">
+        <v>9464051235</v>
+      </c>
+      <c r="B3" s="66">
+        <v>20470</v>
+      </c>
+      <c r="C3" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="69" t="s">
+        <v>165</v>
+      </c>
+      <c r="F3" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H3" s="57">
+        <v>202101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="51">
+        <v>297043676</v>
+      </c>
+      <c r="B4" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="C4" s="58" t="s">
         <v>169</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="D4" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H4" s="58">
+        <v>202101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="51">
+        <v>297044729</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" s="58" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="63" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="55" t="s">
-        <v>154</v>
-      </c>
-      <c r="F1" s="63" t="s">
+      <c r="D5" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H5" s="58">
+        <v>202101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="51">
+        <v>297043919</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="58" t="s">
         <v>171</v>
       </c>
-      <c r="G1" s="63" t="s">
+      <c r="D6" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H6" s="58">
+        <v>202101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="51">
+        <v>297045105</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="58" t="s">
         <v>172</v>
       </c>
-      <c r="H1" s="63" t="s">
+      <c r="D7" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F7" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H7" s="58">
+        <v>202101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="51">
+        <v>297044133</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="58" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="56">
-        <v>9464051154</v>
-      </c>
-      <c r="B2" s="69">
-        <v>20470</v>
-      </c>
-      <c r="C2" s="58" t="s">
+      <c r="D8" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F8" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H8" s="58">
+        <v>202101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="51">
+        <v>239926030</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="58" t="s">
         <v>174</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D9" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="73" t="s">
+      <c r="E9" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F9" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H9" s="58">
+        <v>202101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="52">
+        <v>297046349</v>
+      </c>
+      <c r="B10" s="52">
+        <v>20074</v>
+      </c>
+      <c r="C10" s="59" t="s">
         <v>175</v>
       </c>
-      <c r="F2" s="69" t="s">
+      <c r="D10" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="58" t="s">
+      <c r="E10" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="F10" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H10" s="59">
+        <v>202101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="51">
+        <v>297046500</v>
+      </c>
+      <c r="B11" s="51">
+        <v>20172</v>
+      </c>
+      <c r="C11" s="58" t="s">
         <v>176</v>
       </c>
-      <c r="H2" s="58">
+      <c r="D11" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F11" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H11" s="58">
         <v>202101</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="57">
-        <v>9464051235</v>
-      </c>
-      <c r="B3" s="69">
-        <v>20470</v>
-      </c>
-      <c r="C3" s="59" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="51">
+        <v>297047078</v>
+      </c>
+      <c r="B12" s="51">
+        <v>20626</v>
+      </c>
+      <c r="C12" s="58" t="s">
         <v>177</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D12" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="72" t="s">
-        <v>175</v>
-      </c>
-      <c r="F3" s="70" t="s">
+      <c r="E12" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H3" s="59">
+      <c r="G12" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H12" s="58">
         <v>202101</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="53">
-        <v>297043676</v>
-      </c>
-      <c r="B4" s="53" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="51">
+        <v>2095067686</v>
+      </c>
+      <c r="B13" s="51">
+        <v>20069</v>
+      </c>
+      <c r="C13" s="58" t="s">
         <v>178</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="D13" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F13" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H13" s="58">
+        <v>202101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="51">
+        <v>249707942</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" s="58" t="s">
         <v>179</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D14" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F4" s="60" t="s">
+      <c r="E14" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F14" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H4" s="60">
+      <c r="G14" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H14" s="58">
         <v>202101</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="53">
-        <v>297044729</v>
-      </c>
-      <c r="B5" s="53" t="s">
-        <v>178</v>
-      </c>
-      <c r="C5" s="60" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="51">
+        <v>207654522</v>
+      </c>
+      <c r="B15" s="51">
+        <v>20024</v>
+      </c>
+      <c r="C15" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="D15" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F5" s="60" t="s">
+      <c r="E15" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F15" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H5" s="60">
+      <c r="G15" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H15" s="58">
         <v>202101</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="53">
-        <v>297043919</v>
-      </c>
-      <c r="B6" s="53" t="s">
-        <v>178</v>
-      </c>
-      <c r="C6" s="60" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="51">
+        <v>4098868821</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" s="58" t="s">
         <v>181</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D16" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F6" s="60" t="s">
+      <c r="E16" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F16" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H6" s="60">
+      <c r="G16" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H16" s="58">
         <v>202101</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="53">
-        <v>297045105</v>
-      </c>
-      <c r="B7" s="53" t="s">
-        <v>178</v>
-      </c>
-      <c r="C7" s="60" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="51">
+        <v>4098868902</v>
+      </c>
+      <c r="B17" s="51">
+        <v>20050</v>
+      </c>
+      <c r="C17" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D17" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F7" s="60" t="s">
+      <c r="E17" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F17" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H7" s="60">
+      <c r="G17" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H17" s="58">
         <v>202101</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="53">
-        <v>297044133</v>
-      </c>
-      <c r="B8" s="53" t="s">
-        <v>178</v>
-      </c>
-      <c r="C8" s="60" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="51">
+        <v>4098869046</v>
+      </c>
+      <c r="B18" s="51">
+        <v>20127</v>
+      </c>
+      <c r="C18" s="58" t="s">
         <v>183</v>
       </c>
-      <c r="D8" s="60" t="s">
+      <c r="D18" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F8" s="60" t="s">
+      <c r="E18" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F18" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H8" s="60">
+      <c r="G18" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H18" s="58">
         <v>202101</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="53">
-        <v>239926030</v>
-      </c>
-      <c r="B9" s="53" t="s">
-        <v>178</v>
-      </c>
-      <c r="C9" s="60" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="51">
+        <v>4039430785</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C19" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="D9" s="60" t="s">
+      <c r="D19" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F9" s="60" t="s">
+      <c r="E19" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H9" s="60">
+      <c r="G19" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H19" s="58">
         <v>202101</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="54">
-        <v>297046349</v>
-      </c>
-      <c r="B10" s="54">
-        <v>20074</v>
-      </c>
-      <c r="C10" s="61" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="51">
+        <v>207556865</v>
+      </c>
+      <c r="B20" s="51">
+        <v>20015</v>
+      </c>
+      <c r="C20" s="58" t="s">
         <v>185</v>
       </c>
-      <c r="D10" s="61" t="s">
+      <c r="D20" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="54" t="s">
-        <v>175</v>
-      </c>
-      <c r="F10" s="61" t="s">
+      <c r="E20" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F20" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H10" s="61">
+      <c r="G20" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H20" s="58">
         <v>202101</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="53">
-        <v>297046500</v>
-      </c>
-      <c r="B11" s="53">
-        <v>20172</v>
-      </c>
-      <c r="C11" s="60" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="51">
+        <v>206635605</v>
+      </c>
+      <c r="B21" s="51">
+        <v>20494</v>
+      </c>
+      <c r="C21" s="58" t="s">
         <v>186</v>
       </c>
-      <c r="D11" s="60" t="s">
+      <c r="D21" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F11" s="60" t="s">
+      <c r="E21" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F21" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H11" s="60">
+      <c r="G21" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H21" s="58">
         <v>202101</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="53">
-        <v>297047078</v>
-      </c>
-      <c r="B12" s="53">
-        <v>20626</v>
-      </c>
-      <c r="C12" s="60" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="51">
+        <v>213991314</v>
+      </c>
+      <c r="B22" s="51">
+        <v>20228</v>
+      </c>
+      <c r="C22" s="58" t="s">
         <v>187</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D22" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F12" s="60" t="s">
+      <c r="E22" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F22" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H12" s="60">
+      <c r="G22" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H22" s="58">
         <v>202101</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="53">
-        <v>2095067686</v>
-      </c>
-      <c r="B13" s="53">
-        <v>20069</v>
-      </c>
-      <c r="C13" s="60" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="51">
+        <v>6072505779</v>
+      </c>
+      <c r="B23" s="51">
+        <v>20335</v>
+      </c>
+      <c r="C23" s="58" t="s">
         <v>188</v>
       </c>
-      <c r="D13" s="60" t="s">
+      <c r="D23" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F13" s="60" t="s">
+      <c r="E23" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F23" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H13" s="60">
+      <c r="G23" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="H23" s="58">
         <v>202101</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="53">
-        <v>249707942</v>
-      </c>
-      <c r="B14" s="53" t="s">
-        <v>178</v>
-      </c>
-      <c r="C14" s="60" t="s">
-        <v>189</v>
-      </c>
-      <c r="D14" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F14" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H14" s="60">
-        <v>202101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="53">
-        <v>207654522</v>
-      </c>
-      <c r="B15" s="53">
-        <v>20024</v>
-      </c>
-      <c r="C15" s="60" t="s">
-        <v>190</v>
-      </c>
-      <c r="D15" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F15" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H15" s="60">
-        <v>202101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="53">
-        <v>4098868821</v>
-      </c>
-      <c r="B16" s="53" t="s">
-        <v>178</v>
-      </c>
-      <c r="C16" s="60" t="s">
-        <v>191</v>
-      </c>
-      <c r="D16" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F16" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H16" s="60">
-        <v>202101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="53">
-        <v>4098868902</v>
-      </c>
-      <c r="B17" s="53">
-        <v>20050</v>
-      </c>
-      <c r="C17" s="60" t="s">
-        <v>192</v>
-      </c>
-      <c r="D17" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F17" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H17" s="60">
-        <v>202101</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="53">
-        <v>4098869046</v>
-      </c>
-      <c r="B18" s="53">
-        <v>20127</v>
-      </c>
-      <c r="C18" s="60" t="s">
-        <v>193</v>
-      </c>
-      <c r="D18" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F18" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H18" s="60">
-        <v>202101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="53">
-        <v>4039430785</v>
-      </c>
-      <c r="B19" s="53" t="s">
-        <v>178</v>
-      </c>
-      <c r="C19" s="60" t="s">
-        <v>194</v>
-      </c>
-      <c r="D19" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F19" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H19" s="60">
-        <v>202101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="53">
-        <v>207556865</v>
-      </c>
-      <c r="B20" s="53">
-        <v>20015</v>
-      </c>
-      <c r="C20" s="60" t="s">
-        <v>195</v>
-      </c>
-      <c r="D20" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F20" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H20" s="60">
-        <v>202101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="53">
-        <v>206635605</v>
-      </c>
-      <c r="B21" s="53">
-        <v>20494</v>
-      </c>
-      <c r="C21" s="60" t="s">
-        <v>196</v>
-      </c>
-      <c r="D21" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F21" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H21" s="60">
-        <v>202101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="53">
-        <v>213991314</v>
-      </c>
-      <c r="B22" s="53">
-        <v>20228</v>
-      </c>
-      <c r="C22" s="60" t="s">
-        <v>197</v>
-      </c>
-      <c r="D22" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F22" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="H22" s="60">
-        <v>202101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="53">
-        <v>6072505779</v>
-      </c>
-      <c r="B23" s="53">
-        <v>20335</v>
-      </c>
-      <c r="C23" s="60" t="s">
-        <v>198</v>
-      </c>
-      <c r="D23" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="F23" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="60" t="s">
-        <v>176</v>
-      </c>
-      <c r="H23" s="60">
-        <v>202101</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" tooltip="https://www.vivo.com.br/para-empresas" xr:uid="{61D69C7A-C35B-47D8-91E5-8B561BC8641E}"/>
     <hyperlink ref="E3:E23" r:id="rId2" tooltip="https://www.vivo.com.br/para-empresas" display="https://www.vivo.com.br/para-empresas" xr:uid="{32A2B793-0B89-4C26-8BC3-D4E3F0C35926}"/>

</xml_diff>